<commit_message>
[expression] - [`BINARY`]: previous [`encodeBase64`] has been renamed as [`base64encode`] for consistency. - [`BINARY`]: fix the loading of binary file.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_binary_expression.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_binary_expression.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\src\test\resources\unittesting\artifact\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADABB6C-A09B-4C95-AE89-C45C230C256D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505B6BC1-5E06-4AE2-B40D-2514476A9EAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,21 +49,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
@@ -75,16 +66,10 @@
     <t>nexial.pollWaitMs</t>
   </si>
   <si>
-    <t>nexial.failFast</t>
+    <t>0</t>
   </si>
   <si>
-    <t>nexial.textDelim</t>
-  </si>
-  <si>
-    <t>nexial.verbose</t>
-  </si>
-  <si>
-    <t>nexial.openResult</t>
+    <t>nexial.delayBetweenStepsMs</t>
   </si>
 </sst>
 </file>
@@ -582,7 +567,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -595,7 +582,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -603,51 +590,36 @@
     </row>
     <row r="2" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>

</xml_diff>